<commit_message>
Did some preliminary stuff for Prior Therapy Trials dataset
</commit_message>
<xml_diff>
--- a/SMC Challenge 6/eligibility criteria/Dataset1_WBC_Trials_First.xlsx
+++ b/SMC Challenge 6/eligibility criteria/Dataset1_WBC_Trials_First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\ClinicalTrialChallenge\SMC Challenge 6\eligibility criteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C884EE7B-108D-47AD-8C3F-272F52AE13AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F35EE88-B317-4717-A3D4-35DDFA910216}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2707,9 +2707,6 @@
     <t>NCIT</t>
   </si>
   <si>
-    <t>(C8644=1) AND (C51948&lt;=50000) OR (C8644=0)</t>
-  </si>
-  <si>
     <t>(C51948&gt;=3000)</t>
   </si>
   <si>
@@ -2728,10 +2725,13 @@
     <t>(C51948&gt;=2500)</t>
   </si>
   <si>
-    <t>(C25150&gt;=1 AND C25150&lt;10 AND C51948&gt;=50000) OR (C25150&gt;=10 AND C25150&lt;31) OR (C25150&gt;=1 AND C25150&lt;31)  AND (C9277=1 OR C5440=1 OR C15370=1)</t>
-  </si>
-  <si>
     <t>inclusion_indicator</t>
+  </si>
+  <si>
+    <t>(C8644=1) and (C51948&lt;=50000) or (C8644=0)</t>
+  </si>
+  <si>
+    <t>(C25150&gt;=1 and C25150&lt;10 and C51948&gt;=50000) or (C25150&gt;=10 and C25150&lt;31) or (C25150&gt;=1 and C25150&lt;31)  and (C9277=1 or C5440=1 or C15370=1)</t>
   </si>
 </sst>
 </file>
@@ -3151,7 +3151,7 @@
   <dimension ref="A1:G409"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
@@ -3177,7 +3177,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>44</v>
@@ -3366,7 +3366,7 @@
         <v>195</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3571,7 +3571,7 @@
         <v>194</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>886</v>
+        <v>893</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3678,7 +3678,7 @@
         <v>214</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3785,7 +3785,7 @@
         <v>196</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3808,7 +3808,7 @@
         <v>196</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3859,7 +3859,7 @@
         <v>196</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3882,7 +3882,7 @@
         <v>196</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3989,7 +3989,7 @@
         <v>196</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4068,7 +4068,7 @@
         <v>199</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4161,7 +4161,7 @@
         <v>196</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4338,7 +4338,7 @@
         <v>196</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4571,7 +4571,7 @@
         <v>196</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4622,7 +4622,7 @@
         <v>196</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4659,7 +4659,7 @@
         <v>196</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4808,7 +4808,7 @@
         <v>196</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4831,7 +4831,7 @@
         <v>196</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4882,7 +4882,7 @@
         <v>217</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="112" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4975,7 +4975,7 @@
         <v>196</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="118" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5012,7 +5012,7 @@
         <v>196</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5049,7 +5049,7 @@
         <v>196</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5394,7 +5394,7 @@
         <v>196</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="146" spans="1:7" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5459,7 +5459,7 @@
         <v>196</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5678,7 +5678,7 @@
         <v>198</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5715,7 +5715,7 @@
         <v>196</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="167" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5738,7 +5738,7 @@
         <v>198</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5803,7 +5803,7 @@
         <v>196</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5938,7 +5938,7 @@
         <v>196</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6003,7 +6003,7 @@
         <v>196</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6026,7 +6026,7 @@
         <v>196</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6091,7 +6091,7 @@
         <v>196</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6128,7 +6128,7 @@
         <v>196</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6249,7 +6249,7 @@
         <v>198</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6300,7 +6300,7 @@
         <v>196</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="203" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6337,7 +6337,7 @@
         <v>196</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="205" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6416,7 +6416,7 @@
         <v>196</v>
       </c>
       <c r="G209" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="210" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6467,7 +6467,7 @@
         <v>198</v>
       </c>
       <c r="G212" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="213" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6490,7 +6490,7 @@
         <v>202</v>
       </c>
       <c r="G213" s="4" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6541,7 +6541,7 @@
         <v>196</v>
       </c>
       <c r="G216" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="217" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6634,7 +6634,7 @@
         <v>196</v>
       </c>
       <c r="G222" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="223" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6657,7 +6657,7 @@
         <v>196</v>
       </c>
       <c r="G223" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="224" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6694,7 +6694,7 @@
         <v>196</v>
       </c>
       <c r="G225" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="226" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6717,7 +6717,7 @@
         <v>196</v>
       </c>
       <c r="G226" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="227" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6768,7 +6768,7 @@
         <v>196</v>
       </c>
       <c r="G229" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="230" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6791,7 +6791,7 @@
         <v>196</v>
       </c>
       <c r="G230" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="231" spans="1:7" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6856,7 +6856,7 @@
         <v>198</v>
       </c>
       <c r="G234" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="235" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6907,7 +6907,7 @@
         <v>196</v>
       </c>
       <c r="G237" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="238" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6958,7 +6958,7 @@
         <v>196</v>
       </c>
       <c r="G240" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="241" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7009,7 +7009,7 @@
         <v>197</v>
       </c>
       <c r="G243" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="244" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7032,7 +7032,7 @@
         <v>196</v>
       </c>
       <c r="G244" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="245" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7055,7 +7055,7 @@
         <v>198</v>
       </c>
       <c r="G245" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7134,7 +7134,7 @@
         <v>196</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="251" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7157,7 +7157,7 @@
         <v>196</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="252" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7180,7 +7180,7 @@
         <v>196</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="253" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7259,7 +7259,7 @@
         <v>196</v>
       </c>
       <c r="G257" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7520,7 +7520,7 @@
         <v>196</v>
       </c>
       <c r="G275" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="276" spans="1:7" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>